<commit_message>
add: implement readExcelForScan function to locate and update specific cell in Excel file
</commit_message>
<xml_diff>
--- a/excelJSUtil/test.xlsx
+++ b/excelJSUtil/test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299500E1-6FEC-4F71-86D0-43E89EDDB417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA55F60-14A5-4396-BAF4-656DA2D37B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
   <si>
     <t>Col01</t>
   </si>
@@ -26,26 +26,35 @@
     <t>a</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>c</t>
   </si>
   <si>
     <t>d</t>
   </si>
   <si>
-    <t>b</t>
+    <t>scan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,8 +77,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -353,13 +365,10 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -382,7 +391,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -390,7 +399,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,7 +407,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -414,7 +423,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -422,15 +431,15 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
+      <c r="B9" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -446,7 +455,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -454,7 +463,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -462,7 +471,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,7 +487,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +495,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -494,7 +503,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -510,7 +519,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>